<commit_message>
Update Race and Ethnicity charts.xlsx
</commit_message>
<xml_diff>
--- a/COPHS Ethnicity in Montezuma/Race and Ethnicity charts.xlsx
+++ b/COPHS Ethnicity in Montezuma/Race and Ethnicity charts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Single Race Ethnicity" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
   <si>
     <t>Ethnicity</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Pacific Islander / Native Hawaiian</t>
-  </si>
-  <si>
-    <t>Non Hispanic</t>
   </si>
 </sst>
 </file>
@@ -160,27 +157,42 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1">
-                <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:rPr lang="en-US" sz="2400" b="1" i="0" baseline="0">
+                <a:effectLst/>
               </a:rPr>
-              <a:t>Percent</a:t>
+              <a:t>Proportion of hospitalizations by single Race-Ethnicity </a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" b="1" baseline="0">
-                <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+              <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t> of COPHS Patients for Montezuma county and Colorado</a:t>
+              <a:t>for Montezuma county and Colorado</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" b="1">
-              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-              <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12143250961554335"/>
+          <c:y val="4.1928721174004195E-3"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -212,7 +224,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9418775483253276E-2"/>
+          <c:y val="0.12555588570296639"/>
+          <c:w val="0.93520736008627847"/>
+          <c:h val="0.7524665313062282"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -672,7 +694,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41404326031573091"/>
+          <c:y val="0.16564997771504977"/>
+          <c:w val="0.16352762508460028"/>
+          <c:h val="3.5377606101124157E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -736,6 +767,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -790,7 +822,7 @@
               <a:rPr lang="en-US" sz="2400" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>Percent of COPHS Patients that are Hispanic</a:t>
+              <a:t>Proportion of COVID hospitalizations that are Hispanic</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -917,7 +949,7 @@
           <c:x val="4.2161720983009264E-2"/>
           <c:y val="0.17080210334532925"/>
           <c:w val="0.94278009806465191"/>
-          <c:h val="0.77605180795699502"/>
+          <c:h val="0.69357758115287149"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -1064,65 +1096,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Ethnicity!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Non Hispanic</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Ethnicity!$B$1:$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Montezuma</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Colorado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Ethnicity!$B$3:$C$3</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1A17-4F0B-907C-D8C8AA2361F7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1140,45 +1113,12 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1315483392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
@@ -1254,17 +1194,13 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39481698920672276"/>
-          <c:y val="0.22607101947308136"/>
-          <c:w val="0.12275467916535208"/>
+          <c:x val="0.41443940504986926"/>
+          <c:y val="0.22378006872852232"/>
+          <c:w val="0.16016978557128767"/>
           <c:h val="3.8660064399166603E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -1331,6 +1267,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1368,28 +1305,55 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
                 <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:rPr>
-              <a:t>Percent of COPHS Patients by race</a:t>
+              <a:t>Proportion of COVID hospitalizations </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>by Race</a:t>
+            </a:r>
           </a:p>
           <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
                 <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
               </a:rPr>
               <a:t> for Montezuma county and Colorado</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US">
-              <a:effectLst/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1425,7 +1389,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.9161117634018377E-2"/>
+          <c:y val="0.19959797266720969"/>
+          <c:w val="0.93554517364161593"/>
+          <c:h val="0.66894614897275784"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1872,7 +1846,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.41449147323737812"/>
+          <c:y val="0.24273563218390803"/>
+          <c:w val="0.16267503058468055"/>
+          <c:h val="3.8793374966060279E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3604,19 +3587,123 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.01502</cdr:x>
+      <cdr:y>0.93606</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.50454</cdr:x>
+      <cdr:y>0.98323</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="136525" y="5670550"/>
+          <a:ext cx="4448175" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Source: COPHS_Tidy for January 1, 2021 to September 30, 2021.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
+      <xdr:colOff>523874</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3638,7 +3725,47 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.04415</cdr:x>
+      <cdr:y>0.92268</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.52361</cdr:x>
+      <cdr:y>0.97423</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="409574" y="5114925"/>
+          <a:ext cx="4448175" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Source: COPHS_Tidy for January 1, 2021 to September 30, 2021.</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3668,6 +3795,110 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3981450" y="5762625"/>
+          <a:ext cx="4448175" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Source: COPHS_Tidy for January 1, 2021 to September 30, 2021.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3938,8 +4169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4072,7 +4303,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,15 +4336,8 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
@@ -4153,8 +4377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>